<commit_message>
added docs and logo
</commit_message>
<xml_diff>
--- a/Docs/F�retagsplan.xlsx
+++ b/Docs/F�retagsplan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="21075" windowHeight="9780" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="21075" windowHeight="9780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tjänstepaket" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="61">
   <si>
     <t>Inkomster</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>1500kr/mån</t>
+  </si>
+  <si>
+    <t>Inga fallna träd</t>
   </si>
 </sst>
 </file>
@@ -440,8 +443,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="6" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -469,6 +470,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -777,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P66"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,11 +864,11 @@
       <c r="P4" s="6"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="42"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="40"/>
       <c r="E5" s="23" t="s">
         <v>31</v>
       </c>
@@ -886,9 +889,9 @@
       <c r="P5" s="6"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="43"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="45"/>
+      <c r="A6" s="41"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="43"/>
       <c r="E6" s="4" t="s">
         <v>32</v>
       </c>
@@ -909,9 +912,9 @@
       <c r="P6" s="6"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="45"/>
+      <c r="A7" s="41"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="43"/>
       <c r="E7" s="24" t="s">
         <v>33</v>
       </c>
@@ -932,9 +935,9 @@
       <c r="P7" s="6"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="45"/>
+      <c r="A8" s="41"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="43"/>
       <c r="E8" s="4"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -949,9 +952,9 @@
       <c r="P8" s="6"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="45"/>
+      <c r="A9" s="41"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="43"/>
       <c r="E9" s="25" t="s">
         <v>34</v>
       </c>
@@ -972,9 +975,9 @@
       <c r="P9" s="6"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="43"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="45"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="43"/>
       <c r="E10" s="4" t="s">
         <v>35</v>
       </c>
@@ -995,9 +998,9 @@
       <c r="P10" s="6"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="43"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="45"/>
+      <c r="A11" s="41"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="43"/>
       <c r="E11" s="4" t="s">
         <v>26</v>
       </c>
@@ -1018,9 +1021,9 @@
       <c r="P11" s="6"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="43"/>
-      <c r="B12" s="44"/>
-      <c r="C12" s="45"/>
+      <c r="A12" s="41"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="43"/>
       <c r="E12" s="4" t="s">
         <v>27</v>
       </c>
@@ -1041,9 +1044,9 @@
       <c r="P12" s="6"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
-      <c r="B13" s="44"/>
-      <c r="C13" s="45"/>
+      <c r="A13" s="41"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="43"/>
       <c r="E13" s="4" t="s">
         <v>29</v>
       </c>
@@ -1064,9 +1067,9 @@
       <c r="P13" s="6"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="43"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="45"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="43"/>
       <c r="E14" s="4" t="s">
         <v>28</v>
       </c>
@@ -1087,9 +1090,9 @@
       <c r="P14" s="6"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="43"/>
-      <c r="B15" s="44"/>
-      <c r="C15" s="45"/>
+      <c r="A15" s="41"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="43"/>
       <c r="E15" s="4"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
@@ -1104,9 +1107,9 @@
       <c r="P15" s="6"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="43"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="45"/>
+      <c r="A16" s="41"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="43"/>
       <c r="E16" s="23" t="s">
         <v>36</v>
       </c>
@@ -1127,11 +1130,11 @@
       <c r="P16" s="6"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="43"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="45"/>
+      <c r="A17" s="41"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="43"/>
       <c r="E17" s="4" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
@@ -1150,9 +1153,9 @@
       <c r="P17" s="6"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="43"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="45"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="43"/>
       <c r="E18" s="24" t="s">
         <v>37</v>
       </c>
@@ -1173,9 +1176,9 @@
       <c r="P18" s="6"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="43"/>
-      <c r="B19" s="44"/>
-      <c r="C19" s="45"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="43"/>
       <c r="E19" s="4"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
@@ -1190,9 +1193,9 @@
       <c r="P19" s="6"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="43"/>
-      <c r="B20" s="44"/>
-      <c r="C20" s="45"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="43"/>
       <c r="E20" s="23" t="s">
         <v>46</v>
       </c>
@@ -1213,9 +1216,9 @@
       <c r="P20" s="6"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="43"/>
-      <c r="B21" s="44"/>
-      <c r="C21" s="45"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="43"/>
       <c r="E21" s="4" t="s">
         <v>25</v>
       </c>
@@ -1236,9 +1239,9 @@
       <c r="P21" s="6"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="43"/>
-      <c r="B22" s="44"/>
-      <c r="C22" s="45"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="43"/>
       <c r="E22" s="4" t="s">
         <v>38</v>
       </c>
@@ -1259,9 +1262,9 @@
       <c r="P22" s="6"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="43"/>
-      <c r="B23" s="44"/>
-      <c r="C23" s="45"/>
+      <c r="A23" s="41"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="43"/>
       <c r="E23" s="4" t="s">
         <v>39</v>
       </c>
@@ -1282,9 +1285,9 @@
       <c r="P23" s="6"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="43"/>
-      <c r="B24" s="44"/>
-      <c r="C24" s="45"/>
+      <c r="A24" s="41"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="43"/>
       <c r="E24" s="4"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
@@ -1299,9 +1302,9 @@
       <c r="P24" s="6"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="43"/>
-      <c r="B25" s="44"/>
-      <c r="C25" s="45"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="43"/>
       <c r="E25" s="4"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
@@ -1316,9 +1319,9 @@
       <c r="P25" s="6"/>
     </row>
     <row r="26" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="46"/>
-      <c r="B26" s="47"/>
-      <c r="C26" s="48"/>
+      <c r="A26" s="44"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="46"/>
       <c r="E26" s="28" t="s">
         <v>14</v>
       </c>
@@ -1933,7 +1936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
@@ -1948,12 +1951,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="39"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="48"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2309,8 +2312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2324,12 +2327,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="39"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="48"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2729,12 +2732,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="39"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="48"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
more work on design and foretagsplan, avtal
</commit_message>
<xml_diff>
--- a/Docs/F�retagsplan.xlsx
+++ b/Docs/F�retagsplan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="21075" windowHeight="9780" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="21075" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="Tjänstepaket" sheetId="2" r:id="rId1"/>
@@ -780,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P66"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1936,7 +1936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>

</xml_diff>